<commit_message>
Tela de cadastro de empresa criada
</commit_message>
<xml_diff>
--- a/Sprint2 Backlog.xlsx
+++ b/Sprint2 Backlog.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCA46C12-D3A8-42E0-B0FD-E466EE2718BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/adc5d2c36552c689/Área de Trabalho/Vlad/Sprint2/Sprint-2/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="207" documentId="8_{FCA46C12-D3A8-42E0-B0FD-E466EE2718BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7118887A-2B58-49A3-BB29-AE8FC3617947}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="26">
   <si>
     <t>Requisito</t>
   </si>
@@ -49,9 +54,6 @@
   </si>
   <si>
     <t>Projetos atualizado no GitHub / Documentação do Projeto Atualizada</t>
-  </si>
-  <si>
-    <t>Sprint 02</t>
   </si>
   <si>
     <t> </t>
@@ -118,7 +120,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,7 +228,7 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -235,22 +237,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -593,10 +595,10 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.140625" style="10" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="10"/>
@@ -604,7 +606,7 @@
     <col min="4" max="5" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -621,286 +623,286 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30.75">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="E2" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="E3" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30.75">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="4" t="s">
+      <c r="B7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30.75">
-      <c r="A8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>6</v>
+      <c r="B8" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="E9" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30.75">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>6</v>
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="26.25" customHeight="1">
-      <c r="A13" s="4" t="s">
+      <c r="B13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="33" customHeight="1">
-      <c r="A14" s="4" t="s">
+      <c r="B14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A15" s="4" t="s">
+      <c r="B15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="39.75" customHeight="1">
-      <c r="A16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>6</v>
+      <c r="B16" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E16" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="22.5" customHeight="1">
+    <row r="17" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>6</v>
+        <v>25</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E17" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -909,5 +911,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>